<commit_message>
pdfs and new xls tables
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/AppendixIII.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/AppendixIII.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/fb170/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32BB772-3E28-8248-84E8-CB5408AD726B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11332FF-E496-EC47-A095-960FC289C37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25940" yWindow="460" windowWidth="21320" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>yeat</t>
-  </si>
-  <si>
     <t>open_bed_t</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>total_check</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,19 +453,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>